<commit_message>
Cart Logo and User Logout Button
</commit_message>
<xml_diff>
--- a/Resources/Inventory.xlsx
+++ b/Resources/Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dayan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silve\Documents\GitHub\NIT-Lucky-9-Capstone\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26DB532-5090-41CF-8D30-992F59A7DA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1B23F2-9095-47C7-971E-C0B97162650A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6588" yWindow="468" windowWidth="19944" windowHeight="10368" xr2:uid="{2F6D9572-7642-423D-9845-41866DBF6F52}"/>
+    <workbookView xWindow="6585" yWindow="465" windowWidth="19950" windowHeight="10365" xr2:uid="{2F6D9572-7642-423D-9845-41866DBF6F52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,8 +305,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$₱-464]#,##0.00;[Red][$₱-464]#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -342,13 +342,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,886 +666,887 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>150</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>9011188511100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>9011188511101</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>120</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>9011188511102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>200</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>9011188511103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>180</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>9011188511104</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>150</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>9011188511105</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>80</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>9011188511106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>9011188511107</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>70</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>9011188511108</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>9011188511109</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>90</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>9011188511110</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>120</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>9011188511111</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>9011188511112</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>150</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>9011188511113</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <v>60</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>9011188511114</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>200</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>9011188511115</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <v>350</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>9011188511116</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>300</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>9011188511117</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="4">
         <v>600</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>9011188511118</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <v>500</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>9011188511119</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>9011188511120</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>9011188511121</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="4">
         <v>35</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>9011188511122</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="4">
         <v>80</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>9011188511123</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="4">
         <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <v>9011188511124</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
         <v>250</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>9011188511125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <v>70</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>9011188511126</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <v>35</v>
       </c>
       <c r="D29" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>9011188511127</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="4">
         <v>250</v>
       </c>
       <c r="D30" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>9011188511128</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
       <c r="B31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <v>50</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>9011188511129</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="4">
         <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>9011188511130</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
       <c r="B33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <v>35</v>
       </c>
       <c r="D33" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>9011188511131</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
       <c r="B34" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>9011188511132</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
       <c r="B35" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="4">
         <v>120</v>
       </c>
       <c r="D35" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>9011188511133</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="B36" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <v>60</v>
       </c>
       <c r="D36" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>9011188511134</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>46</v>
       </c>
       <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="4">
         <v>150</v>
       </c>
       <c r="D37" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>9011188511135</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="4">
         <v>80</v>
       </c>
       <c r="D38" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>9011188511136</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="4">
         <v>90</v>
       </c>
       <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>9011188511137</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>49</v>
       </c>
       <c r="B40" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="4">
         <v>15</v>
       </c>
       <c r="D40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>9011188511138</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>50</v>
       </c>
       <c r="B41" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="4">
         <v>25</v>
       </c>
       <c r="D41" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>9011188511139</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="4">
         <v>200</v>
       </c>
       <c r="D42" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>9011188511140</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
       <c r="B43" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="4">
         <v>250</v>
       </c>
       <c r="D43" t="s">
         <v>51</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>9011188511141</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="4">
         <v>80</v>
       </c>
       <c r="D44" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>9011188511142</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
       <c r="B45" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="4">
         <v>150</v>
       </c>
       <c r="D45" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="3">
         <v>9011188511143</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="4">
         <v>120</v>
       </c>
       <c r="D46" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="3">
         <v>9011188511144</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="4">
         <v>60</v>
       </c>
       <c r="D47" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="3">
         <v>9011188511145</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="4">
         <v>100</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="3">
         <v>9011188511146</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
       <c r="B49" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="4">
         <v>30</v>
       </c>
       <c r="D49" t="s">
         <v>57</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="3">
         <v>9011188511147</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
       <c r="B50" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="4">
         <v>50</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="3">
         <v>9011188511148</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
       <c r="B51" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="4">
         <v>70</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="3">
         <v>9011188511149</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>